<commit_message>
correction of SubRES_SUP_Techs.xlsx - Biorefiniry not available until 2020
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SUP_Techs.xlsx
+++ b/SubRES_TMPL/SubRES_SUP_Techs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="1365" windowWidth="17940" windowHeight="9855"/>
+    <workbookView xWindow="1455" yWindow="1365" windowWidth="17940" windowHeight="9855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SUP_BioRefineries" sheetId="6" r:id="rId1"/>
@@ -10898,8 +10898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -11251,7 +11251,7 @@
         <v>70</v>
       </c>
       <c r="H15" s="26">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="I15" s="27">
         <v>0.23809523809523808</v>
@@ -11702,8 +11702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Final fixes - Applied demand named FUEL, POWER and HET - fixed mistaken WPE to WCH
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SUP_Techs.xlsx
+++ b/SubRES_TMPL/SubRES_SUP_Techs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="1365" windowWidth="17940" windowHeight="9855" activeTab="1"/>
+    <workbookView xWindow="1455" yWindow="1365" windowWidth="17940" windowHeight="9855"/>
   </bookViews>
   <sheets>
     <sheet name="SUP_BioRefineries" sheetId="6" r:id="rId1"/>
@@ -1146,7 +1146,7 @@
     <t>Miscellaneous indexes</t>
   </si>
   <si>
-    <t>WPE</t>
+    <t>WCH</t>
   </si>
 </sst>
 </file>
@@ -10898,8 +10898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U51"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -11702,8 +11702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>